<commit_message>
Changed back to .NET 4.5.2. Updates in polish reports.
</commit_message>
<xml_diff>
--- a/Sprawozdanie.xlsx
+++ b/Sprawozdanie.xlsx
@@ -5740,8 +5740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P217" sqref="P217"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>